<commit_message>
removed conc_, change docs
</commit_message>
<xml_diff>
--- a/example/data_ap_major_volatile.xlsx
+++ b/example/data_ap_major_volatile.xlsx
@@ -5,17 +5,29 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexweiranli/Downloads/new/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/easonzz/Documents/GitHub/pyAp/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D93E21-A36F-964F-98FA-0E00B3996C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADAA0C3-D76D-AE48-BB78-4A510BF153C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="25260" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="500" windowWidth="25260" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -490,7 +502,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>